<commit_message>
updated excel file phone column to text and String in RegistrationPage class
</commit_message>
<xml_diff>
--- a/AutomationPractice/src/main/resources/excel/registrationdata.xlsx
+++ b/AutomationPractice/src/main/resources/excel/registrationdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -49,7 +49,10 @@
     <t xml:space="preserve">test</t>
   </si>
   <si>
-    <t xml:space="preserve">user1</t>
+    <t xml:space="preserve">userA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adr123</t>
   </si>
   <si>
     <t xml:space="preserve">Nairobi</t>
@@ -58,18 +61,34 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">user2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user3</t>
+    <t xml:space="preserve">0712345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adr124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0712345679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adr125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0712345680</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -143,12 +162,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,37 +199,39 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:H4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -216,20 +245,20 @@
       <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>12345</v>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1010</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>12345678</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,25 +266,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>12346</v>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1011</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>12345679</v>
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,25 +292,25 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>12347</v>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>1012</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>12345680</v>
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>